<commit_message>
Added plot to generateModel.py
</commit_message>
<xml_diff>
--- a/src/module_1/p6_test results.xlsx
+++ b/src/module_1/p6_test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/faf89f17094f69d9/_School/2024_TU Delft Bsc EE/2025-2026/Q2_EE2L1/Project/src/module_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="8_{FF6D4E3F-F320-4EC6-AC2B-1AEDDC2D4F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34C13317-40C0-4758-9F41-BCBF1E810337}"/>
+  <xr:revisionPtr revIDLastSave="292" documentId="8_{FF6D4E3F-F320-4EC6-AC2B-1AEDDC2D4F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCF0660E-DC61-47ED-9FD8-454D9485BCF8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{27495DE4-06DE-42D5-9603-5AE5B78F0026}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{27495DE4-06DE-42D5-9603-5AE5B78F0026}"/>
   </bookViews>
   <sheets>
     <sheet name="Old config" sheetId="1" r:id="rId1"/>
@@ -286,15 +286,15 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -646,7 +646,7 @@
     <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9.140625" style="1"/>
-    <col min="6" max="11" width="9.140625" style="4"/>
+    <col min="6" max="11" width="9.140625" style="2"/>
     <col min="12" max="17" width="9.140625" style="1"/>
     <col min="18" max="18" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -654,33 +654,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="5"/>
+      <c r="N1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="5"/>
+      <c r="P1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2" t="s">
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="2"/>
+      <c r="S1" s="5"/>
       <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
@@ -701,22 +701,22 @@
       <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>50</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -763,27 +763,27 @@
       <c r="E3" s="1">
         <v>22</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <f>P3</f>
         <v>0</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="2">
         <f>Q3</f>
         <v>0</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="2">
         <f>L3+N3</f>
         <v>10</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="2">
         <f>M3+O3</f>
         <v>7</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="2">
         <f>S3</f>
         <v>0</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="2">
         <f>R3</f>
         <v>0</v>
       </c>
@@ -831,27 +831,27 @@
       <c r="E4" s="1">
         <v>14</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <f t="shared" ref="F4:F26" si="0">P4</f>
         <v>0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="2">
         <f t="shared" ref="G4:G26" si="1">Q4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="2">
         <f t="shared" ref="H4:H26" si="2">L4+N4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="2">
         <f t="shared" ref="I4:I26" si="3">M4+O4</f>
         <v>0</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="2">
         <f t="shared" ref="J4:J26" si="4">S4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="2">
         <f t="shared" ref="K4:K26" si="5">R4</f>
         <v>0</v>
       </c>
@@ -899,27 +899,27 @@
       <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -951,50 +951,50 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="5" t="s">
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1005,27 +1005,27 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1037,27 +1037,27 @@
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1069,27 +1069,27 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1101,27 +1101,27 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1133,27 +1133,27 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1165,27 +1165,27 @@
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1197,27 +1197,27 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1229,27 +1229,27 @@
       <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1261,27 +1261,27 @@
       <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1293,27 +1293,27 @@
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1325,27 +1325,27 @@
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1357,27 +1357,27 @@
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1389,27 +1389,27 @@
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="4">
+      <c r="F19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1421,27 +1421,27 @@
       <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="4">
+      <c r="F20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1453,27 +1453,27 @@
       <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="4">
+      <c r="F21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1485,27 +1485,27 @@
       <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="4">
+      <c r="F22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1517,27 +1517,27 @@
       <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="4">
+      <c r="F23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1549,27 +1549,27 @@
       <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H24" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="4">
+      <c r="F24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1581,27 +1581,27 @@
       <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="4">
+      <c r="F25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1613,36 +1613,36 @@
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H26" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="4">
+      <c r="F26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1667,7 +1667,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1675,7 @@
     <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9.140625" style="1"/>
-    <col min="6" max="11" width="9.140625" style="4"/>
+    <col min="6" max="11" width="9.140625" style="2"/>
     <col min="12" max="17" width="9.140625" style="1"/>
     <col min="18" max="18" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1683,33 +1683,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="5"/>
+      <c r="N1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="5"/>
+      <c r="P1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2" t="s">
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="2"/>
+      <c r="S1" s="5"/>
       <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
@@ -1730,22 +1730,22 @@
       <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>50</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -1792,27 +1792,27 @@
       <c r="E3" s="1">
         <v>20</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <f>P3</f>
         <v>1</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="2">
         <f>Q3</f>
         <v>0</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="2">
         <f>L3+N3</f>
         <v>8</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="2">
         <f>M3+O3</f>
         <v>8</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="2">
         <f>S3</f>
         <v>0</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="2">
         <f>R3</f>
         <v>0</v>
       </c>
@@ -1860,27 +1860,27 @@
       <c r="E4" s="1">
         <v>21</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <f t="shared" ref="F4:G26" si="0">P4</f>
         <v>0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="2">
         <f t="shared" ref="H4:I26" si="1">L4+N4</f>
         <v>10</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="2">
         <f t="shared" ref="J4:J26" si="2">S4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="2">
         <f t="shared" ref="K4:K26" si="3">R4</f>
         <v>0</v>
       </c>
@@ -1928,27 +1928,27 @@
       <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1996,27 +1996,27 @@
       <c r="E6" s="1">
         <v>12</v>
       </c>
-      <c r="F6" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="J6" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
+      <c r="J6" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2064,27 +2064,27 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2116,49 +2116,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2167,29 +2167,65 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="C9" s="1">
+        <v>108</v>
+      </c>
+      <c r="D9" s="1">
+        <v>104</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1">
+        <v>2</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -2199,29 +2235,65 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="C10" s="1">
+        <v>106</v>
+      </c>
+      <c r="D10" s="1">
+        <v>98</v>
+      </c>
+      <c r="E10" s="1">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>3</v>
+      </c>
+      <c r="O10" s="1">
+        <v>3</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -2231,27 +2303,27 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2263,27 +2335,27 @@
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="4">
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2295,27 +2367,27 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2327,27 +2399,27 @@
       <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2359,27 +2431,27 @@
       <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2391,27 +2463,27 @@
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2423,27 +2495,27 @@
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="4">
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2455,27 +2527,27 @@
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="4">
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2487,27 +2559,27 @@
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="4">
+      <c r="F19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2519,27 +2591,27 @@
       <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="4">
+      <c r="F20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2551,27 +2623,27 @@
       <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="4">
+      <c r="F21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2583,27 +2655,27 @@
       <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="4">
+      <c r="F22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2615,27 +2687,27 @@
       <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="4">
+      <c r="F23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2647,27 +2719,27 @@
       <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H24" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="4">
+      <c r="F24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2679,27 +2751,27 @@
       <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="4">
+      <c r="F25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2711,48 +2783,49 @@
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H26" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="4">
+      <c r="F26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="2" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="R1:S1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated GUI to TUI
</commit_message>
<xml_diff>
--- a/src/module_1/p6_test results.xlsx
+++ b/src/module_1/p6_test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/faf89f17094f69d9/_School/2024_TU Delft Bsc EE/2025-2026/Q2_EE2L1/Project/src/module_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="292" documentId="8_{FF6D4E3F-F320-4EC6-AC2B-1AEDDC2D4F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCF0660E-DC61-47ED-9FD8-454D9485BCF8}"/>
+  <xr:revisionPtr revIDLastSave="326" documentId="8_{FF6D4E3F-F320-4EC6-AC2B-1AEDDC2D4F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AC64E0E-B107-485D-8C5D-72BCC6DF6B3D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{27495DE4-06DE-42D5-9603-5AE5B78F0026}"/>
   </bookViews>
@@ -1664,10 +1664,10 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2303,6 +2303,15 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
+      <c r="C11" s="1">
+        <v>102</v>
+      </c>
+      <c r="D11" s="1">
+        <v>102</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2327,38 +2336,77 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2367,6 +2415,15 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
+      <c r="C13" s="1">
+        <v>102</v>
+      </c>
+      <c r="D13" s="1">
+        <v>102</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2391,38 +2448,91 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="C14" s="4">
+        <v>24</v>
+      </c>
+      <c r="D14" s="4">
+        <v>19</v>
+      </c>
+      <c r="E14" s="4">
+        <v>83</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>78</v>
+      </c>
+      <c r="M14" s="4">
+        <v>5</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>73</v>
+      </c>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">

</xml_diff>